<commit_message>
금요일 SP를 30 => 20
</commit_message>
<xml_diff>
--- a/Excel/Invasion.xlsx
+++ b/Excel/Invasion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectNoname\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09488264-B6A2-42E5-AAD1-92FE40FA26EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EFE5A6-121B-403D-B74C-D7CC5956BF47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DB6A53DD-5DCE-4DDC-8DA5-FDED601CA3A9}"/>
   </bookViews>
@@ -1581,7 +1581,7 @@
         <v>53</v>
       </c>
       <c r="L27">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
@@ -1616,7 +1616,7 @@
         <v>54</v>
       </c>
       <c r="L28">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
@@ -1651,7 +1651,7 @@
         <v>55</v>
       </c>
       <c r="L29">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
@@ -1686,7 +1686,7 @@
         <v>56</v>
       </c>
       <c r="L30">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
@@ -1721,7 +1721,7 @@
         <v>57</v>
       </c>
       <c r="L31">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>